<commit_message>
plotted the numbers for random graphs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laplacian\TreePCG\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25598" windowHeight="15900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -108,6 +113,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -436,20 +449,20 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.3125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1875" customWidth="1"/>
+    <col min="4" max="4" width="16.8125" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="11" max="11" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17">
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -516,7 +529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="E7" s="1"/>
     </row>
   </sheetData>

</xml_diff>